<commit_message>
feat: adicionando 2.3C - 3 a planilha unificada
</commit_message>
<xml_diff>
--- a/PlanilhaUnificada.xlsx
+++ b/PlanilhaUnificada.xlsx
@@ -8,28 +8,36 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\trabalhoPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E55F874-1E8C-497F-9DB0-5AE434367C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DFBC7A-AB7B-47F5-B243-7C28FEF8CD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2.3A" sheetId="3" r:id="rId1"/>
     <sheet name="2.3E-8" sheetId="4" r:id="rId2"/>
+    <sheet name="2.3C-3" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'2.3A'!$B$19:$H$19</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'2.3C-3'!$B$22:$O$22</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'2.3E-8'!$B$11:$G$11</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'2.3A'!$B$19:$E$19</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'2.3C-3'!$P$3:$P$21</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'2.3E-8'!$H$10</definedName>
     <definedName name="solver_lhs10" localSheetId="0" hidden="1">'2.3A'!$K$18</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'2.3A'!$B$19:$E$19</definedName>
@@ -49,28 +57,40 @@
     <definedName name="solver_lhs9" localSheetId="0" hidden="1">'2.3A'!$I$16</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_msl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">10</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">8</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'2.3A'!$I$2</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'2.3C-3'!$R$21</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'2.3E-8'!$H$2</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel10" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">1</definedName>
@@ -89,6 +109,7 @@
     <definedName name="solver_rel8" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel9" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'2.3A'!$K$3:$K$6</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'2.3C-3'!$R$3:$R$21</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">'2.3E-8'!$J$10</definedName>
     <definedName name="solver_rhs10" localSheetId="0" hidden="1">'2.3A'!$K$17</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">'2.3A'!$K$11:$K$14</definedName>
@@ -107,24 +128,34 @@
     <definedName name="solver_rhs8" localSheetId="1" hidden="1">'2.3E-8'!$J$9</definedName>
     <definedName name="solver_rhs9" localSheetId="0" hidden="1">'2.3A'!$K$16</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_rsd" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.01</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.01</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -159,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="92">
   <si>
     <t>PROBLEMA</t>
   </si>
@@ -333,13 +364,115 @@
   </si>
   <si>
     <t>Razão de mistura A/B II</t>
+  </si>
+  <si>
+    <t>Valores</t>
+  </si>
+  <si>
+    <t>Valor do empréstimo Z-1</t>
+  </si>
+  <si>
+    <t>Valor do empréstimo Z-2</t>
+  </si>
+  <si>
+    <t>Valor do empréstimo Z-3</t>
+  </si>
+  <si>
+    <t>Valor do empréstimo Z-4</t>
+  </si>
+  <si>
+    <t>Participação Total P1-1</t>
+  </si>
+  <si>
+    <t>Participação Total P2-1</t>
+  </si>
+  <si>
+    <t>Participação Total P1-2</t>
+  </si>
+  <si>
+    <t>Participação Total P2-2</t>
+  </si>
+  <si>
+    <t>Participação Total P1-3</t>
+  </si>
+  <si>
+    <t>Participação Total P2-3</t>
+  </si>
+  <si>
+    <t>Participação Total P1-4</t>
+  </si>
+  <si>
+    <t>Participação Total P2-4</t>
+  </si>
+  <si>
+    <t>Participação Total P1-5</t>
+  </si>
+  <si>
+    <t>Participação Total P2-5</t>
+  </si>
+  <si>
+    <t>Valor total P1</t>
+  </si>
+  <si>
+    <t>Valor total P2</t>
+  </si>
+  <si>
+    <t>Valor total P3</t>
+  </si>
+  <si>
+    <t>Valor total P4</t>
+  </si>
+  <si>
+    <t>Valor total P5</t>
+  </si>
+  <si>
+    <t>P1-1</t>
+  </si>
+  <si>
+    <t>P2-1</t>
+  </si>
+  <si>
+    <t>Z-1</t>
+  </si>
+  <si>
+    <t>P1-2</t>
+  </si>
+  <si>
+    <t>P2-2</t>
+  </si>
+  <si>
+    <t>Z-2</t>
+  </si>
+  <si>
+    <t>P1-3</t>
+  </si>
+  <si>
+    <t>P2-3</t>
+  </si>
+  <si>
+    <t>Z-3</t>
+  </si>
+  <si>
+    <t>P1-4</t>
+  </si>
+  <si>
+    <t>P2-4</t>
+  </si>
+  <si>
+    <t>Z-4</t>
+  </si>
+  <si>
+    <t>P1-5</t>
+  </si>
+  <si>
+    <t>P2-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -422,6 +555,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -455,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -483,6 +629,8 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
     </xf>
@@ -493,7 +641,12 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="2" tint="-0.24994659260841701"/>
@@ -782,8 +935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A36C73D-5DDD-4F70-818B-6E24CF2FC329}">
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection sqref="A1:M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -867,14 +1020,14 @@
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="N2" s="15" t="s">
+      <c r="N2" s="17" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="3"/>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="16"/>
+      <c r="Q2" s="18"/>
       <c r="R2" t="e">
         <f ca="1">_xludf.MIN($I$2)</f>
         <v>#NAME?</v>
@@ -914,12 +1067,12 @@
       <c r="K3" s="6">
         <v>100</v>
       </c>
-      <c r="N3" s="15"/>
+      <c r="N3" s="17"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="16" t="s">
+      <c r="P3" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="16"/>
+      <c r="Q3" s="18"/>
       <c r="R3">
         <f>COUNT($B$19:$H$19)</f>
         <v>7</v>
@@ -959,12 +1112,12 @@
       <c r="K4" s="6">
         <v>125</v>
       </c>
-      <c r="N4" s="15"/>
+      <c r="N4" s="17"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="16"/>
+      <c r="Q4" s="18"/>
       <c r="R4" t="b">
         <f t="array" ref="R4">$B$19:$E$19&gt;=$K$3:$K$6</f>
         <v>1</v>
@@ -1004,12 +1157,12 @@
       <c r="K5" s="6">
         <v>75</v>
       </c>
-      <c r="N5" s="15"/>
+      <c r="N5" s="17"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="16"/>
+      <c r="Q5" s="18"/>
       <c r="R5" t="b">
         <f t="array" ref="R5">$B$19:$E$19&lt;=$K$11:$K$14</f>
         <v>1</v>
@@ -1049,12 +1202,12 @@
       <c r="K6" s="6">
         <v>300</v>
       </c>
-      <c r="N6" s="15"/>
+      <c r="N6" s="17"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="16"/>
+      <c r="Q6" s="18"/>
       <c r="R6" t="b">
         <f t="array" ref="R6">$B$19:$H$19=INT($B$19:$H$19)</f>
         <v>1</v>
@@ -1094,10 +1247,10 @@
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="15"/>
+      <c r="N7" s="17"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="16"/>
-      <c r="Q7" s="16"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
       <c r="R7" t="b">
         <f>$F$19=$K$8</f>
         <v>1</v>
@@ -1138,12 +1291,12 @@
         <f>(1.3*$B$19+1.2*$C$19+0.5*$D$19+1.4*$E$19)/25</f>
         <v>35</v>
       </c>
-      <c r="N8" s="15"/>
+      <c r="N8" s="17"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="16"/>
+      <c r="Q8" s="18"/>
       <c r="R8" t="b">
         <f>$G$19&lt;=$K$15</f>
         <v>1</v>
@@ -1184,12 +1337,12 @@
         <f>0.023*B19+0.034*C19+0.046*D19+0.023*E19</f>
         <v>25</v>
       </c>
-      <c r="N9" s="15"/>
+      <c r="N9" s="17"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="16"/>
+      <c r="Q9" s="18"/>
       <c r="R9" t="b">
         <f>$G$19=$K$9</f>
         <v>1</v>
@@ -1229,7 +1382,7 @@
       <c r="K10" s="6">
         <v>200</v>
       </c>
-      <c r="N10" s="15"/>
+      <c r="N10" s="17"/>
       <c r="O10" s="3"/>
       <c r="R10" t="b">
         <f>$G$19&gt;=$K$7</f>
@@ -1270,7 +1423,7 @@
       <c r="K11" s="6">
         <v>200</v>
       </c>
-      <c r="N11" s="15"/>
+      <c r="N11" s="17"/>
       <c r="O11" s="3"/>
       <c r="R11" t="b">
         <f>$H$19&lt;=$K$10</f>
@@ -1311,7 +1464,7 @@
       <c r="K12" s="6">
         <v>190</v>
       </c>
-      <c r="N12" s="15" t="s">
+      <c r="N12" s="17" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="3"/>
@@ -1354,7 +1507,7 @@
       <c r="K13" s="6">
         <v>260</v>
       </c>
-      <c r="N13" s="15"/>
+      <c r="N13" s="17"/>
       <c r="O13" s="3"/>
       <c r="R13" t="b">
         <f>$K$18&lt;=$K$17</f>
@@ -1395,7 +1548,7 @@
       <c r="K14" s="6">
         <v>600</v>
       </c>
-      <c r="N14" s="15"/>
+      <c r="N14" s="17"/>
       <c r="O14" s="3"/>
       <c r="R14">
         <f>{32767;32767;0.000001;0.01;TRUE;FALSE;TRUE;1;1;1;0.0001;TRUE}</f>
@@ -1436,7 +1589,7 @@
       <c r="K15" s="6">
         <v>25</v>
       </c>
-      <c r="N15" s="15"/>
+      <c r="N15" s="17"/>
       <c r="O15" s="3"/>
       <c r="R15">
         <f>{0;0;2;100;0;FALSE;TRUE;0.075;0;0;FALSE;30}</f>
@@ -1477,7 +1630,7 @@
       <c r="K16" s="6">
         <v>2</v>
       </c>
-      <c r="N16" s="15"/>
+      <c r="N16" s="17"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1515,7 +1668,7 @@
         <f>0.85*(50+(H19*H17))</f>
         <v>42.5</v>
       </c>
-      <c r="N17" s="15"/>
+      <c r="N17" s="17"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1553,7 +1706,7 @@
         <f>B18*B19+C18*C19+D18*D19+E18*E19+F18*F19+G18*G19</f>
         <v>34.44</v>
       </c>
-      <c r="N18" s="15"/>
+      <c r="N18" s="17"/>
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1581,23 +1734,23 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="N19" s="15"/>
+      <c r="N19" s="17"/>
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N20" s="15"/>
+      <c r="N20" s="17"/>
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N21" s="15"/>
+      <c r="N21" s="17"/>
       <c r="O21" s="3"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N22" s="15"/>
+      <c r="N22" s="17"/>
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N23" s="15" t="s">
+      <c r="N23" s="17" t="s">
         <v>4</v>
       </c>
       <c r="O23" s="4"/>
@@ -1607,7 +1760,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="N24" s="15"/>
+      <c r="N24" s="17"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
@@ -1628,7 +1781,7 @@
     <mergeCell ref="P7:Q7"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:H16">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1641,8 +1794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{263368B4-FA2B-4D67-BCBF-3F3EBFF15146}">
   <dimension ref="A1:K15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,6 +2217,1267 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:G11">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D899204E-A298-4429-B21E-01E72C42F145}">
+  <dimension ref="A1:S22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="15">
+        <v>-1</v>
+      </c>
+      <c r="C2" s="15">
+        <v>-3</v>
+      </c>
+      <c r="D2" s="15">
+        <v>1</v>
+      </c>
+      <c r="E2" s="15">
+        <v>-3.1</v>
+      </c>
+      <c r="F2" s="15">
+        <v>-2.5</v>
+      </c>
+      <c r="G2" s="15">
+        <v>1</v>
+      </c>
+      <c r="H2" s="15">
+        <v>-1.5</v>
+      </c>
+      <c r="I2" s="15">
+        <v>1.5</v>
+      </c>
+      <c r="J2" s="15">
+        <v>1</v>
+      </c>
+      <c r="K2" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="L2" s="15">
+        <v>1.8</v>
+      </c>
+      <c r="M2" s="15">
+        <v>1</v>
+      </c>
+      <c r="N2" s="15">
+        <v>5</v>
+      </c>
+      <c r="O2" s="15">
+        <v>2.8</v>
+      </c>
+      <c r="P2">
+        <f t="array" ref="P2:P21">MMULT(B2:O21,TRANSPOSE(B22:O22))</f>
+        <v>12.899999999999999</v>
+      </c>
+      <c r="S2" t="e">
+        <f ca="1">_xludf.MAX($R$21)</f>
+        <v>#NAME?</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <f>COUNT($B$22:$O$22)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <f t="array" ref="S4">$P$3:$P$21&lt;=$R$3:$R$21</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>12</v>
+      </c>
+      <c r="R5">
+        <v>1</v>
+      </c>
+      <c r="S5">
+        <f>{32767;32767;0.000001;0.01;FALSE;FALSE;TRUE;1;1;1;0.0001;TRUE}</f>
+        <v>32767</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
+      </c>
+      <c r="S6">
+        <f>{0;0;1;100;0;FALSE;TRUE;0.075;0;0;FALSE;30}</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>12</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>1</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>0</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>12</v>
+      </c>
+      <c r="R14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>1</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>12</v>
+      </c>
+      <c r="R15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>3</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R17">
+        <f>D22*D2+1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>3.1</v>
+      </c>
+      <c r="F18">
+        <v>2.5</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>0</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R18">
+        <f>(R17-P17)*1.0173+1-(1.0182*D22*D2)</f>
+        <v>2.0173000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>3.1</v>
+      </c>
+      <c r="F19">
+        <v>2.5</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>1.5</v>
+      </c>
+      <c r="I19">
+        <v>-1.5</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>-1.5</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19">
+        <f>(R18-P18)*1.0173+1-(1.0182*G22*G2)</f>
+        <v>3.0521992900000003</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <v>3</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>3.1</v>
+      </c>
+      <c r="F20">
+        <v>2.5</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1.5</v>
+      </c>
+      <c r="I20">
+        <v>-1.5</v>
+      </c>
+      <c r="J20">
+        <v>0</v>
+      </c>
+      <c r="K20">
+        <v>-1.8</v>
+      </c>
+      <c r="L20">
+        <v>-1.8</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>-5.0999999999999996</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>12</v>
+      </c>
+      <c r="R20">
+        <f>(R19-P19)*1.0173+1-(1.0182*J22*J2)</f>
+        <v>5.6309523377170017</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>3.1</v>
+      </c>
+      <c r="F21">
+        <v>2.5</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1.5</v>
+      </c>
+      <c r="I21">
+        <v>-1.5</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>-1.8</v>
+      </c>
+      <c r="L21">
+        <v>-1.8</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>-5</v>
+      </c>
+      <c r="O21">
+        <v>-2.8</v>
+      </c>
+      <c r="P21">
+        <v>-12.899999999999999</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>12</v>
+      </c>
+      <c r="R21">
+        <f>-(P21)+1+(R20-P20)*1.0173-(1.0182*M22*M2)</f>
+        <v>24.816597813159504</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>0</v>
+      </c>
+      <c r="N22">
+        <v>1</v>
+      </c>
+      <c r="O22">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="12" type="noConversion"/>
+  <conditionalFormatting sqref="B3:O21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
feat: mudando cor da solução
</commit_message>
<xml_diff>
--- a/PlanilhaUnificada.xlsx
+++ b/PlanilhaUnificada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\trabalhoPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1DFBC7A-AB7B-47F5-B243-7C28FEF8CD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF4A874B-8C81-456C-A048-ED179930D43F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -520,13 +520,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="14"/>
       <color theme="0"/>
@@ -564,6 +557,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -620,16 +621,15 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="justify"/>
@@ -637,6 +637,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1020,14 +1021,14 @@
       </c>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
-      <c r="N2" s="17" t="s">
+      <c r="N2" s="16" t="s">
         <v>5</v>
       </c>
       <c r="O2" s="3"/>
-      <c r="P2" s="18" t="s">
+      <c r="P2" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="18"/>
+      <c r="Q2" s="17"/>
       <c r="R2" t="e">
         <f ca="1">_xludf.MIN($I$2)</f>
         <v>#NAME?</v>
@@ -1067,12 +1068,12 @@
       <c r="K3" s="6">
         <v>100</v>
       </c>
-      <c r="N3" s="17"/>
+      <c r="N3" s="16"/>
       <c r="O3" s="3"/>
-      <c r="P3" s="18" t="s">
+      <c r="P3" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="Q3" s="18"/>
+      <c r="Q3" s="17"/>
       <c r="R3">
         <f>COUNT($B$19:$H$19)</f>
         <v>7</v>
@@ -1112,12 +1113,12 @@
       <c r="K4" s="6">
         <v>125</v>
       </c>
-      <c r="N4" s="17"/>
+      <c r="N4" s="16"/>
       <c r="O4" s="3"/>
-      <c r="P4" s="18" t="s">
+      <c r="P4" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="Q4" s="18"/>
+      <c r="Q4" s="17"/>
       <c r="R4" t="b">
         <f t="array" ref="R4">$B$19:$E$19&gt;=$K$3:$K$6</f>
         <v>1</v>
@@ -1157,12 +1158,12 @@
       <c r="K5" s="6">
         <v>75</v>
       </c>
-      <c r="N5" s="17"/>
+      <c r="N5" s="16"/>
       <c r="O5" s="3"/>
-      <c r="P5" s="18" t="s">
+      <c r="P5" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="18"/>
+      <c r="Q5" s="17"/>
       <c r="R5" t="b">
         <f t="array" ref="R5">$B$19:$E$19&lt;=$K$11:$K$14</f>
         <v>1</v>
@@ -1202,12 +1203,12 @@
       <c r="K6" s="6">
         <v>300</v>
       </c>
-      <c r="N6" s="17"/>
+      <c r="N6" s="16"/>
       <c r="O6" s="3"/>
-      <c r="P6" s="18" t="s">
+      <c r="P6" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="Q6" s="18"/>
+      <c r="Q6" s="17"/>
       <c r="R6" t="b">
         <f t="array" ref="R6">$B$19:$H$19=INT($B$19:$H$19)</f>
         <v>1</v>
@@ -1247,10 +1248,10 @@
       <c r="K7" s="6">
         <v>0</v>
       </c>
-      <c r="N7" s="17"/>
+      <c r="N7" s="16"/>
       <c r="O7" s="3"/>
-      <c r="P7" s="18"/>
-      <c r="Q7" s="18"/>
+      <c r="P7" s="17"/>
+      <c r="Q7" s="17"/>
       <c r="R7" t="b">
         <f>$F$19=$K$8</f>
         <v>1</v>
@@ -1291,12 +1292,12 @@
         <f>(1.3*$B$19+1.2*$C$19+0.5*$D$19+1.4*$E$19)/25</f>
         <v>35</v>
       </c>
-      <c r="N8" s="17"/>
+      <c r="N8" s="16"/>
       <c r="O8" s="3"/>
-      <c r="P8" s="18" t="s">
+      <c r="P8" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="Q8" s="18"/>
+      <c r="Q8" s="17"/>
       <c r="R8" t="b">
         <f>$G$19&lt;=$K$15</f>
         <v>1</v>
@@ -1337,12 +1338,12 @@
         <f>0.023*B19+0.034*C19+0.046*D19+0.023*E19</f>
         <v>25</v>
       </c>
-      <c r="N9" s="17"/>
+      <c r="N9" s="16"/>
       <c r="O9" s="3"/>
-      <c r="P9" s="18" t="s">
+      <c r="P9" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="Q9" s="18"/>
+      <c r="Q9" s="17"/>
       <c r="R9" t="b">
         <f>$G$19=$K$9</f>
         <v>1</v>
@@ -1382,7 +1383,7 @@
       <c r="K10" s="6">
         <v>200</v>
       </c>
-      <c r="N10" s="17"/>
+      <c r="N10" s="16"/>
       <c r="O10" s="3"/>
       <c r="R10" t="b">
         <f>$G$19&gt;=$K$7</f>
@@ -1423,7 +1424,7 @@
       <c r="K11" s="6">
         <v>200</v>
       </c>
-      <c r="N11" s="17"/>
+      <c r="N11" s="16"/>
       <c r="O11" s="3"/>
       <c r="R11" t="b">
         <f>$H$19&lt;=$K$10</f>
@@ -1464,7 +1465,7 @@
       <c r="K12" s="6">
         <v>190</v>
       </c>
-      <c r="N12" s="17" t="s">
+      <c r="N12" s="16" t="s">
         <v>3</v>
       </c>
       <c r="O12" s="3"/>
@@ -1507,7 +1508,7 @@
       <c r="K13" s="6">
         <v>260</v>
       </c>
-      <c r="N13" s="17"/>
+      <c r="N13" s="16"/>
       <c r="O13" s="3"/>
       <c r="R13" t="b">
         <f>$K$18&lt;=$K$17</f>
@@ -1548,7 +1549,7 @@
       <c r="K14" s="6">
         <v>600</v>
       </c>
-      <c r="N14" s="17"/>
+      <c r="N14" s="16"/>
       <c r="O14" s="3"/>
       <c r="R14">
         <f>{32767;32767;0.000001;0.01;TRUE;FALSE;TRUE;1;1;1;0.0001;TRUE}</f>
@@ -1589,7 +1590,7 @@
       <c r="K15" s="6">
         <v>25</v>
       </c>
-      <c r="N15" s="17"/>
+      <c r="N15" s="16"/>
       <c r="O15" s="3"/>
       <c r="R15">
         <f>{0;0;2;100;0;FALSE;TRUE;0.075;0;0;FALSE;30}</f>
@@ -1630,7 +1631,7 @@
       <c r="K16" s="6">
         <v>2</v>
       </c>
-      <c r="N16" s="17"/>
+      <c r="N16" s="16"/>
       <c r="O16" s="3"/>
     </row>
     <row r="17" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1668,7 +1669,7 @@
         <f>0.85*(50+(H19*H17))</f>
         <v>42.5</v>
       </c>
-      <c r="N17" s="17"/>
+      <c r="N17" s="16"/>
       <c r="O17" s="3"/>
     </row>
     <row r="18" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1706,7 +1707,7 @@
         <f>B18*B19+C18*C19+D18*D19+E18*E19+F18*F19+G18*G19</f>
         <v>34.44</v>
       </c>
-      <c r="N18" s="17"/>
+      <c r="N18" s="16"/>
       <c r="O18" s="3"/>
     </row>
     <row r="19" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
@@ -1734,23 +1735,23 @@
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
       <c r="K19" s="6"/>
-      <c r="N19" s="17"/>
+      <c r="N19" s="16"/>
       <c r="O19" s="3"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N20" s="17"/>
+      <c r="N20" s="16"/>
       <c r="O20" s="3"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N21" s="17"/>
+      <c r="N21" s="16"/>
       <c r="O21" s="3"/>
     </row>
     <row r="22" spans="1:15" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N22" s="17"/>
+      <c r="N22" s="16"/>
       <c r="O22" s="3"/>
     </row>
     <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="N23" s="17" t="s">
+      <c r="N23" s="16" t="s">
         <v>4</v>
       </c>
       <c r="O23" s="4"/>
@@ -1760,7 +1761,7 @@
       <c r="C24" s="6"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
-      <c r="N24" s="17"/>
+      <c r="N24" s="16"/>
     </row>
     <row r="25" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B25" s="6"/>
@@ -1795,7 +1796,7 @@
   <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1843,19 +1844,19 @@
       <c r="C2" s="10">
         <v>10</v>
       </c>
-      <c r="D2" s="14">
-        <v>0</v>
-      </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
-        <v>0</v>
-      </c>
-      <c r="G2" s="14">
-        <v>0</v>
-      </c>
-      <c r="H2" s="13">
+      <c r="D2" s="13">
+        <v>0</v>
+      </c>
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
+        <v>0</v>
+      </c>
+      <c r="G2" s="13">
+        <v>0</v>
+      </c>
+      <c r="H2" s="18">
         <f t="array" ref="H2:H10">MMULT(B2:G10,TRANSPOSE(B11:G11))</f>
         <v>10031.91489361702</v>
       </c>
@@ -1886,7 +1887,7 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="18">
         <v>450.00000000000011</v>
       </c>
       <c r="I3" t="s">
@@ -1922,7 +1923,7 @@
       <c r="G4">
         <v>1</v>
       </c>
-      <c r="H4" s="13">
+      <c r="H4" s="18">
         <v>700</v>
       </c>
       <c r="I4" t="s">
@@ -1958,7 +1959,7 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="18">
         <v>428.72340425532821</v>
       </c>
       <c r="I5" t="s">
@@ -1994,7 +1995,7 @@
       <c r="G6">
         <v>89</v>
       </c>
-      <c r="H6" s="13">
+      <c r="H6" s="18">
         <v>3.637978807091713E-12</v>
       </c>
       <c r="I6" t="s">
@@ -2030,7 +2031,7 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="18">
         <v>-1644.6808510638289</v>
       </c>
       <c r="I7" t="s">
@@ -2066,7 +2067,7 @@
       <c r="G8">
         <v>8</v>
       </c>
-      <c r="H8" s="13">
+      <c r="H8" s="18">
         <v>4.5474735088646412E-13</v>
       </c>
       <c r="I8" t="s">
@@ -2102,7 +2103,7 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="18">
         <v>5.6843418860808015E-14</v>
       </c>
       <c r="I9" t="s">
@@ -2138,7 +2139,7 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10" s="13">
+      <c r="H10" s="18">
         <v>0</v>
       </c>
       <c r="I10" t="s">
@@ -2230,7 +2231,7 @@
   <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2295,49 +2296,49 @@
       <c r="A2" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>-1</v>
       </c>
-      <c r="C2" s="15">
+      <c r="C2" s="14">
         <v>-3</v>
       </c>
-      <c r="D2" s="15">
-        <v>1</v>
-      </c>
-      <c r="E2" s="15">
+      <c r="D2" s="14">
+        <v>1</v>
+      </c>
+      <c r="E2" s="14">
         <v>-3.1</v>
       </c>
-      <c r="F2" s="15">
+      <c r="F2" s="14">
         <v>-2.5</v>
       </c>
-      <c r="G2" s="15">
-        <v>1</v>
-      </c>
-      <c r="H2" s="15">
+      <c r="G2" s="14">
+        <v>1</v>
+      </c>
+      <c r="H2" s="14">
         <v>-1.5</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <v>1.5</v>
       </c>
-      <c r="J2" s="15">
-        <v>1</v>
-      </c>
-      <c r="K2" s="15">
+      <c r="J2" s="14">
+        <v>1</v>
+      </c>
+      <c r="K2" s="14">
         <v>1.8</v>
       </c>
-      <c r="L2" s="15">
+      <c r="L2" s="14">
         <v>1.8</v>
       </c>
-      <c r="M2" s="15">
-        <v>1</v>
-      </c>
-      <c r="N2" s="15">
+      <c r="M2" s="14">
+        <v>1</v>
+      </c>
+      <c r="N2" s="14">
         <v>5</v>
       </c>
-      <c r="O2" s="15">
+      <c r="O2" s="14">
         <v>2.8</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="18">
         <f t="array" ref="P2:P21">MMULT(B2:O21,TRANSPOSE(B22:O22))</f>
         <v>12.899999999999999</v>
       </c>
@@ -2392,7 +2393,7 @@
       <c r="O3">
         <v>0</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="18">
         <v>0</v>
       </c>
       <c r="Q3" t="s">
@@ -2452,7 +2453,7 @@
       <c r="O4">
         <v>0</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="18">
         <v>0</v>
       </c>
       <c r="Q4" t="s">
@@ -2512,7 +2513,7 @@
       <c r="O5">
         <v>0</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="18">
         <v>0</v>
       </c>
       <c r="Q5" t="s">
@@ -2572,7 +2573,7 @@
       <c r="O6">
         <v>0</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="18">
         <v>0</v>
       </c>
       <c r="Q6" t="s">
@@ -2632,7 +2633,7 @@
       <c r="O7">
         <v>0</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="18">
         <v>0</v>
       </c>
       <c r="Q7" t="s">
@@ -2688,10 +2689,10 @@
       <c r="O8">
         <v>0</v>
       </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="16" t="s">
+      <c r="P8" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="15" t="s">
         <v>12</v>
       </c>
       <c r="R8">
@@ -2744,10 +2745,10 @@
       <c r="O9">
         <v>0</v>
       </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="16" t="s">
+      <c r="P9" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="15" t="s">
         <v>12</v>
       </c>
       <c r="R9">
@@ -2800,10 +2801,10 @@
       <c r="O10">
         <v>0</v>
       </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10" s="16" t="s">
+      <c r="P10" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="15" t="s">
         <v>12</v>
       </c>
       <c r="R10">
@@ -2856,10 +2857,10 @@
       <c r="O11">
         <v>0</v>
       </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="16" t="s">
+      <c r="P11" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="15" t="s">
         <v>12</v>
       </c>
       <c r="R11">
@@ -2912,10 +2913,10 @@
       <c r="O12">
         <v>0</v>
       </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="16" t="s">
+      <c r="P12" s="18">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="15" t="s">
         <v>12</v>
       </c>
       <c r="R12">
@@ -2968,7 +2969,7 @@
       <c r="O13">
         <v>0</v>
       </c>
-      <c r="P13">
+      <c r="P13" s="18">
         <v>1</v>
       </c>
       <c r="Q13" t="s">
@@ -3024,7 +3025,7 @@
       <c r="O14">
         <v>0</v>
       </c>
-      <c r="P14">
+      <c r="P14" s="18">
         <v>1</v>
       </c>
       <c r="Q14" t="s">
@@ -3080,7 +3081,7 @@
       <c r="O15">
         <v>0</v>
       </c>
-      <c r="P15">
+      <c r="P15" s="18">
         <v>1</v>
       </c>
       <c r="Q15" t="s">
@@ -3136,7 +3137,7 @@
       <c r="O16">
         <v>1</v>
       </c>
-      <c r="P16">
+      <c r="P16" s="18">
         <v>1</v>
       </c>
       <c r="Q16" t="s">
@@ -3192,10 +3193,10 @@
       <c r="O17">
         <v>0</v>
       </c>
-      <c r="P17">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="16" t="s">
+      <c r="P17" s="18">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="15" t="s">
         <v>12</v>
       </c>
       <c r="R17">
@@ -3249,7 +3250,7 @@
       <c r="O18">
         <v>0</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="18">
         <v>0</v>
       </c>
       <c r="Q18" t="s">
@@ -3306,7 +3307,7 @@
       <c r="O19">
         <v>0</v>
       </c>
-      <c r="P19">
+      <c r="P19" s="18">
         <v>-1.5</v>
       </c>
       <c r="Q19" t="s">
@@ -3363,7 +3364,7 @@
       <c r="O20">
         <v>0</v>
       </c>
-      <c r="P20">
+      <c r="P20" s="18">
         <v>-5.0999999999999996</v>
       </c>
       <c r="Q20" t="s">
@@ -3420,7 +3421,7 @@
       <c r="O21">
         <v>-2.8</v>
       </c>
-      <c r="P21">
+      <c r="P21" s="18">
         <v>-12.899999999999999</v>
       </c>
       <c r="Q21" t="s">
@@ -3476,7 +3477,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="12" type="noConversion"/>
+  <phoneticPr fontId="11" type="noConversion"/>
   <conditionalFormatting sqref="B3:O21">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>

</xml_diff>